<commit_message>
Update west balkans data
</commit_message>
<xml_diff>
--- a/DataCollection.xlsx
+++ b/DataCollection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Documents/World Bank/Projects/EPM_APPLIED/EPM_WestBalkans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDDDEFD-0EAD-9547-99A4-B7D8FC6CD133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6248A62-55BA-9A46-BA5D-E9CA9B037A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25760" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <r>
       <t>Category</t>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>Bosnia &amp; Herzgovina</t>
+  </si>
+  <si>
+    <t>ENTSOE</t>
+  </si>
+  <si>
+    <t>CCDR</t>
+  </si>
+  <si>
+    <t>None - perfect market assumption</t>
   </si>
 </sst>
 </file>
@@ -477,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -527,16 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
@@ -579,6 +579,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,15 +945,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" style="33" customWidth="1"/>
     <col min="6" max="6" width="36.83203125" style="14" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
@@ -949,38 +961,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -989,8 +1001,10 @@
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="19"/>
+      <c r="E4" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="16"/>
       <c r="G4" s="6" t="b">
         <v>0</v>
       </c>
@@ -1000,25 +1014,27 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="34"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20"/>
+      <c r="E5" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="17"/>
       <c r="G5" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1027,90 +1043,96 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="19"/>
       <c r="G6" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="34"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="17"/>
       <c r="G7" s="6" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="34"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="19"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="34"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="6" t="b">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="34"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="19"/>
+      <c r="E10" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="29"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1119,72 +1141,74 @@
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="17"/>
       <c r="G11" s="6" t="b">
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="34"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="19"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="34"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="32"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="34"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="I14" s="29"/>
     </row>
     <row r="15" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1193,72 +1217,72 @@
       <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="20"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="32"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="34"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="19"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="32"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="34"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="20"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="32"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="34"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="19"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="10" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="32"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="30" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1267,33 +1291,33 @@
       <c r="D19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="20"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="29"/>
+      <c r="I19" s="26"/>
     </row>
     <row r="20" spans="2:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="35"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="21"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="30"/>
+      <c r="I20" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1308,28 +1332,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82d385a5-b9a6-4475-856d-5007da75fd0b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050C578EB5D77054695BB39CED13AE195" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b13242139522a6682c8c86fafa67dfe0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="82d385a5-b9a6-4475-856d-5007da75fd0b" xmlns:ns3="136f07d9-b196-48f3-8d9c-1b68f2918d71" xmlns:ns4="3e02667f-0271-471b-bd6e-11a2e16def1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="160c33603bfd62138bfa0e3f67cfac52" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1606,27 +1608,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B76B34E3-5368-4422-91E9-C8C7E71F56D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82d385a5-b9a6-4475-856d-5007da75fd0b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D055469-B72E-4028-9AB3-692F36F813E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="82d385a5-b9a6-4475-856d-5007da75fd0b"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E50AC05B-6DAB-4622-ADDB-77347ACBD0B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1645,4 +1649,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D055469-B72E-4028-9AB3-692F36F813E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="82d385a5-b9a6-4475-856d-5007da75fd0b"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B76B34E3-5368-4422-91E9-C8C7E71F56D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>